<commit_message>
Intento adjuntar archivo, no funciona y dejo comentado el codigo.
</commit_message>
<xml_diff>
--- a/templates/rentabilidades.xlsx
+++ b/templates/rentabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Desktop/AccuMails/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C614FED4-10F2-8D49-BF27-4288CD78F905}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0295AF5-7C56-3F4C-AF2C-08F57640414D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>EMAIL</t>
   </si>
@@ -52,13 +52,7 @@
     <t>ACCOUNT</t>
   </si>
   <si>
-    <t>Igor</t>
-  </si>
-  <si>
     <t>Jose</t>
-  </si>
-  <si>
-    <t>ialonso@accuratequant.com</t>
   </si>
 </sst>
 </file>
@@ -69,7 +63,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,14 +194,6 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -510,7 +496,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -554,9 +540,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -570,11 +555,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -606,7 +588,6 @@
     <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="43" builtinId="8"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Millares" xfId="42" builtinId="3"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -930,20 +911,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="27.83203125" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
-    <col min="7" max="8" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="3" max="9" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -977,7 +955,7 @@
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1004,39 +982,7 @@
         <v>28.58</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>61192.49</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>46250</v>
-      </c>
-      <c r="G3" s="1">
-        <v>28681.87</v>
-      </c>
-      <c r="H3" s="1">
-        <v>13739.380000000001</v>
-      </c>
-      <c r="I3" s="3">
-        <v>28.58</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{CECEF19C-2FAC-0540-B2BB-5A8201EC2CDB}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio en email template de rentabilidades
</commit_message>
<xml_diff>
--- a/templates/rentabilidades.xlsx
+++ b/templates/rentabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Desktop/AccuMails/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0295AF5-7C56-3F4C-AF2C-08F57640414D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9A65DB-BC25-F54E-A6A2-C2A222C56C05}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -914,7 +914,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>